<commit_message>
starting to edit codebook
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BPatel\Documents\GitHub\Data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E332E95D-C5CD-497E-BC6C-89E6A63C3873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6007A336-1709-4AB5-9FFC-0F365F6766F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="545" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="codebook" sheetId="2" r:id="rId1"/>
-    <sheet name="fair4rsv1.0Instructions" sheetId="7" r:id="rId2"/>
-    <sheet name="fair4rsv1.0InstructionsCategory" sheetId="8" r:id="rId3"/>
-    <sheet name="reviewStrategy" sheetId="1" r:id="rId4"/>
-    <sheet name="resourcesList" sheetId="4" r:id="rId5"/>
-    <sheet name="resourcesReview" sheetId="5" r:id="rId6"/>
-    <sheet name="resourcesReviewKeywords" sheetId="6" r:id="rId7"/>
+    <sheet name="codebook new" sheetId="9" r:id="rId2"/>
+    <sheet name="fair4rsv1.0Instructions" sheetId="7" r:id="rId3"/>
+    <sheet name="fair4rsv1.0InstructionsCategory" sheetId="8" r:id="rId4"/>
+    <sheet name="reviewStrategy" sheetId="1" r:id="rId5"/>
+    <sheet name="resourcesList" sheetId="4" r:id="rId6"/>
+    <sheet name="resourcesReview" sheetId="5" r:id="rId7"/>
+    <sheet name="resourcesReviewKeywords" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2996" uniqueCount="985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3011" uniqueCount="986">
   <si>
     <t>reviewCategory</t>
   </si>
@@ -3323,6 +3324,9 @@
   </si>
   <si>
     <t>SciCrunch</t>
+  </si>
+  <si>
+    <t>fair4rsv1.0Instructions</t>
   </si>
 </sst>
 </file>
@@ -3513,6 +3517,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3527,9 +3534,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3814,8 +3818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754C8F5D-D1F8-4C3C-916A-C26AC74F8087}">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView zoomScale="52" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5036,11 +5040,97 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2427A3B1-0328-4098-ADF9-6D0FBB76AA04}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>985</v>
+      </c>
+      <c r="B2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>985</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868A66FF-FB53-4D7D-93AD-C2CA3F6CAE27}">
   <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5052,20 +5142,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>591</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="28" t="s">
         <v>573</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
@@ -5101,20 +5191,20 @@
       <c r="A7" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="29" t="s">
         <v>626</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="31" t="s">
         <v>580</v>
       </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="31"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
@@ -5150,16 +5240,16 @@
       <c r="A13" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="32" t="s">
         <v>586</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="32"/>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="31" t="s">
         <v>582</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="31"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
@@ -5195,16 +5285,16 @@
       <c r="A19" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="32" t="s">
         <v>587</v>
       </c>
-      <c r="C19" s="31"/>
+      <c r="C19" s="32"/>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="31" t="s">
         <v>583</v>
       </c>
-      <c r="C21" s="30"/>
+      <c r="C21" s="31"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
@@ -5240,16 +5330,16 @@
       <c r="A25" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="32" t="s">
         <v>635</v>
       </c>
-      <c r="C25" s="31"/>
+      <c r="C25" s="32"/>
     </row>
     <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="31" t="s">
         <v>585</v>
       </c>
-      <c r="C27" s="30"/>
+      <c r="C27" s="31"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B28" s="10" t="s">
@@ -5285,16 +5375,16 @@
       <c r="A31" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="32" t="s">
         <v>637</v>
       </c>
-      <c r="C31" s="31"/>
+      <c r="C31" s="32"/>
     </row>
     <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="31" t="s">
         <v>589</v>
       </c>
-      <c r="C33" s="30"/>
+      <c r="C33" s="31"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B34" s="10" t="s">
@@ -5328,22 +5418,22 @@
       <c r="A37" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="32" t="s">
         <v>636</v>
       </c>
-      <c r="C37" s="31"/>
+      <c r="C37" s="32"/>
     </row>
     <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="30" t="s">
         <v>592</v>
       </c>
-      <c r="C39" s="29"/>
+      <c r="C39" s="30"/>
     </row>
     <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="28" t="s">
         <v>593</v>
       </c>
-      <c r="C41" s="27"/>
+      <c r="C41" s="28"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B42" s="8" t="s">
@@ -5379,16 +5469,16 @@
       <c r="A45" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="29" t="s">
         <v>630</v>
       </c>
-      <c r="C45" s="28"/>
+      <c r="C45" s="29"/>
     </row>
     <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="28" t="s">
         <v>596</v>
       </c>
-      <c r="C47" s="27"/>
+      <c r="C47" s="28"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B48" s="8" t="s">
@@ -5424,16 +5514,16 @@
       <c r="A51" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="29" t="s">
         <v>598</v>
       </c>
-      <c r="C51" s="28"/>
+      <c r="C51" s="29"/>
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="28" t="s">
         <v>599</v>
       </c>
-      <c r="C53" s="27"/>
+      <c r="C53" s="28"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B54" s="8" t="s">
@@ -5469,16 +5559,16 @@
       <c r="A57" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="29" t="s">
         <v>627</v>
       </c>
-      <c r="C57" s="28"/>
+      <c r="C57" s="29"/>
     </row>
     <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59" s="27" t="s">
+      <c r="B59" s="28" t="s">
         <v>601</v>
       </c>
-      <c r="C59" s="27"/>
+      <c r="C59" s="28"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B60" s="8" t="s">
@@ -5514,26 +5604,26 @@
       <c r="A63" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B63" s="28" t="s">
+      <c r="B63" s="29" t="s">
         <v>628</v>
       </c>
-      <c r="C63" s="28"/>
+      <c r="C63" s="29"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
     </row>
     <row r="65" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B65" s="29" t="s">
+      <c r="B65" s="30" t="s">
         <v>604</v>
       </c>
-      <c r="C65" s="29"/>
+      <c r="C65" s="30"/>
     </row>
     <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B67" s="27" t="s">
+      <c r="B67" s="28" t="s">
         <v>605</v>
       </c>
-      <c r="C67" s="27"/>
+      <c r="C67" s="28"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B68" s="8" t="s">
@@ -5569,16 +5659,16 @@
       <c r="A71" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B71" s="28" t="s">
+      <c r="B71" s="29" t="s">
         <v>629</v>
       </c>
-      <c r="C71" s="28"/>
+      <c r="C71" s="29"/>
     </row>
     <row r="73" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B73" s="27" t="s">
+      <c r="B73" s="28" t="s">
         <v>608</v>
       </c>
-      <c r="C73" s="27"/>
+      <c r="C73" s="28"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B74" s="8" t="s">
@@ -5614,22 +5704,22 @@
       <c r="A77" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B77" s="28" t="s">
+      <c r="B77" s="29" t="s">
         <v>631</v>
       </c>
-      <c r="C77" s="28"/>
+      <c r="C77" s="29"/>
     </row>
     <row r="79" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B79" s="29" t="s">
+      <c r="B79" s="30" t="s">
         <v>610</v>
       </c>
-      <c r="C79" s="29"/>
+      <c r="C79" s="30"/>
     </row>
     <row r="81" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B81" s="27" t="s">
+      <c r="B81" s="28" t="s">
         <v>611</v>
       </c>
-      <c r="C81" s="27"/>
+      <c r="C81" s="28"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B82" s="8" t="s">
@@ -5665,16 +5755,16 @@
       <c r="A85" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B85" s="28" t="s">
+      <c r="B85" s="29" t="s">
         <v>632</v>
       </c>
-      <c r="C85" s="28"/>
+      <c r="C85" s="29"/>
     </row>
     <row r="87" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B87" s="27" t="s">
+      <c r="B87" s="28" t="s">
         <v>612</v>
       </c>
-      <c r="C87" s="27"/>
+      <c r="C87" s="28"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B88" s="8" t="s">
@@ -5710,16 +5800,16 @@
       <c r="A91" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B91" s="28" t="s">
+      <c r="B91" s="29" t="s">
         <v>633</v>
       </c>
-      <c r="C91" s="28"/>
+      <c r="C91" s="29"/>
     </row>
     <row r="93" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B93" s="27" t="s">
+      <c r="B93" s="28" t="s">
         <v>613</v>
       </c>
-      <c r="C93" s="27"/>
+      <c r="C93" s="28"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B94" s="8" t="s">
@@ -5755,16 +5845,16 @@
       <c r="A97" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B97" s="28" t="s">
+      <c r="B97" s="29" t="s">
         <v>618</v>
       </c>
-      <c r="C97" s="28"/>
+      <c r="C97" s="29"/>
     </row>
     <row r="99" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B99" s="27" t="s">
+      <c r="B99" s="28" t="s">
         <v>614</v>
       </c>
-      <c r="C99" s="27"/>
+      <c r="C99" s="28"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B100" s="8" t="s">
@@ -5798,16 +5888,16 @@
       <c r="A103" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B103" s="28" t="s">
+      <c r="B103" s="29" t="s">
         <v>634</v>
       </c>
-      <c r="C103" s="28"/>
+      <c r="C103" s="29"/>
     </row>
     <row r="105" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B105" s="27" t="s">
+      <c r="B105" s="28" t="s">
         <v>619</v>
       </c>
-      <c r="C105" s="27"/>
+      <c r="C105" s="28"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B106" s="8" t="s">
@@ -5843,35 +5933,13 @@
       <c r="A109" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B109" s="28" t="s">
+      <c r="B109" s="29" t="s">
         <v>621</v>
       </c>
-      <c r="C109" s="28"/>
+      <c r="C109" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B47:C47"/>
     <mergeCell ref="B99:C99"/>
     <mergeCell ref="B103:C103"/>
     <mergeCell ref="B105:C105"/>
@@ -5888,13 +5956,35 @@
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B91:C91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3402B4BF-7BA0-4B6A-ADE0-C35D566CD98E}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -6024,7 +6114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
@@ -6308,7 +6398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49D82B-1314-44E9-9C10-AF21C213EB48}">
   <dimension ref="A1:G314"/>
   <sheetViews>
@@ -13574,7 +13664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{594EE843-E3DA-42D6-9C6E-79F5CD2EA4F7}">
   <dimension ref="A1:AC71"/>
   <sheetViews>
@@ -16820,11 +16910,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0221B120-414C-4095-AF2A-591768752CFE}">
   <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="S5" sqref="S5"/>
@@ -17051,7 +17141,7 @@
       <c r="S3" s="15" t="s">
         <v>982</v>
       </c>
-      <c r="X3" s="32" t="s">
+      <c r="X3" s="27" t="s">
         <v>983</v>
       </c>
     </row>

</xml_diff>